<commit_message>
Replacing excel activitiesfor Hospitality account file
</commit_message>
<xml_diff>
--- a/GPO Roster Avendra_Dispatcher/Data/Config.xlsx
+++ b/GPO Roster Avendra_Dispatcher/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubSai\GPO-Roster-Avendra\GPO Roster Avendra_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D19A4DE-7EDF-424B-8B57-788FC73429C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7C72E4-9A25-4A96-A32A-F601C6130616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -315,7 +315,7 @@
     <t>Avendra_Columns</t>
   </si>
   <si>
-    <t>Prod</t>
+    <t>Dev</t>
   </si>
 </sst>
 </file>
@@ -711,7 +711,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1794,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z986"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -3072,7 +3072,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3127,6 +3127,9 @@
       <c r="B2" t="s">
         <v>77</v>
       </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
       <c r="D2" t="s">
         <v>74</v>
       </c>
@@ -3138,6 +3141,9 @@
       <c r="B3" t="s">
         <v>59</v>
       </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
@@ -3146,6 +3152,9 @@
       <c r="B4" t="s">
         <v>67</v>
       </c>
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
@@ -3154,6 +3163,9 @@
       <c r="B5" t="s">
         <v>68</v>
       </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
@@ -3162,6 +3174,9 @@
       <c r="B6" t="s">
         <v>78</v>
       </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
@@ -3170,6 +3185,9 @@
       <c r="B7" t="s">
         <v>79</v>
       </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
@@ -3178,6 +3196,9 @@
       <c r="B8" t="s">
         <v>80</v>
       </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
@@ -3186,6 +3207,9 @@
       <c r="B9" t="s">
         <v>73</v>
       </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
@@ -3194,6 +3218,9 @@
       <c r="B10" t="s">
         <v>76</v>
       </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
       <c r="D10" t="s">
         <v>92</v>
       </c>
@@ -3205,6 +3232,9 @@
       <c r="B11" t="s">
         <v>89</v>
       </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
@@ -3213,6 +3243,9 @@
       <c r="B12" t="s">
         <v>93</v>
       </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
@@ -3220,6 +3253,9 @@
       </c>
       <c r="B13" t="s">
         <v>95</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Latest Code Update - March'25
</commit_message>
<xml_diff>
--- a/GPO Roster Avendra_Dispatcher/Data/Config.xlsx
+++ b/GPO Roster Avendra_Dispatcher/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubSai\GPO-Roster-Avendra\GPO Roster Avendra_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7C72E4-9A25-4A96-A32A-F601C6130616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89C076D-28A6-4166-B2D3-E2B202A9ECF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -315,7 +315,7 @@
     <t>Avendra_Columns</t>
   </si>
   <si>
-    <t>Dev</t>
+    <t>Prod</t>
   </si>
 </sst>
 </file>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3071,8 +3071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Increase in download timeout
</commit_message>
<xml_diff>
--- a/GPO Roster Avendra_Dispatcher/Data/Config.xlsx
+++ b/GPO Roster Avendra_Dispatcher/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubAnkush\GPO-Roster-Avendra\GPO Roster Avendra_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubSai\GPO-Roster-Avendra\GPO Roster Avendra_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA09E6B-2BAD-449F-9585-87AB58638396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFA9C09-AB47-443A-BC5A-FBDA45D97FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>ERP</t>
+  </si>
+  <si>
+    <t>DownloadTimeOut_GPOAvendra</t>
+  </si>
+  <si>
+    <t>DownloadTimeOut</t>
   </si>
   <si>
     <t>Prod</t>
@@ -711,15 +717,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -767,19 +773,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1794,16 +1800,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z986"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="72.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1840,7 +1846,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1851,7 +1857,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1965,7 +1971,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -3072,16 +3078,16 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C2" sqref="C2:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="4" width="72.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="4" width="72.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3127,6 +3133,9 @@
       <c r="B2" t="s">
         <v>76</v>
       </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
       <c r="D2" t="s">
         <v>73</v>
       </c>
@@ -3138,6 +3147,9 @@
       <c r="B3" t="s">
         <v>59</v>
       </c>
+      <c r="C3" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
@@ -3146,6 +3158,9 @@
       <c r="B4" t="s">
         <v>67</v>
       </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
@@ -3154,6 +3169,9 @@
       <c r="B5" t="s">
         <v>68</v>
       </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
@@ -3162,6 +3180,9 @@
       <c r="B6" t="s">
         <v>77</v>
       </c>
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
@@ -3170,6 +3191,9 @@
       <c r="B7" t="s">
         <v>78</v>
       </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
@@ -3178,6 +3202,9 @@
       <c r="B8" t="s">
         <v>79</v>
       </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
@@ -3186,6 +3213,9 @@
       <c r="B9" t="s">
         <v>72</v>
       </c>
+      <c r="C9" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
@@ -3194,6 +3224,9 @@
       <c r="B10" t="s">
         <v>75</v>
       </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
       <c r="D10" t="s">
         <v>91</v>
       </c>
@@ -3205,6 +3238,9 @@
       <c r="B11" t="s">
         <v>88</v>
       </c>
+      <c r="C11" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
@@ -3213,6 +3249,9 @@
       <c r="B12" t="s">
         <v>92</v>
       </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
@@ -3221,8 +3260,21 @@
       <c r="B13" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" t="s">
+        <v>98</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>